<commit_message>
updated boards and BoM.  added PTCs, changed to molex connectors, and updated diode and other componenets.
</commit_message>
<xml_diff>
--- a/design/schematics/arm_motor_controller/BOM.xlsx
+++ b/design/schematics/arm_motor_controller/BOM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finge\Documents\GitHub\agse\design\schematics\arm_motor_controller\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t>PART</t>
   </si>
@@ -39,9 +44,6 @@
     <t>Polarized Capacitor</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/Panasonic/EEE-1HA101UP/?qs=sGAEpiMZZMsh%252b1woXyUXj5yjySvXixb0PHeYiLMejMg%3d</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
@@ -66,15 +68,9 @@
     <t>D1</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Diode-SMA</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/STMicroelectronics/STTH5R06GY-TR/?qs=sGAEpiMZZMtoHjESLttvkp8idLYzK2a8ecDhIjQRqPo%3d</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -207,27 +203,6 @@
     <t>http://www.mouser.com/ProductDetail/Vishay/CRCW080550R0FKTA/?qs=aRXG1QX2Yl9J6LSLM7CpJQ%3d%3d</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>370 RESISTOR</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>1.5K RESISTOR</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-2RKF1501X/?qs=sGAEpiMZZMvdGkrng054t8AJgcdMkx7xOyRawAAbetk%3d</t>
-  </si>
-  <si>
-    <t>3.5mm Screw Terminal</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/8084</t>
-  </si>
-  <si>
     <t>Molex 4 Wire Jumper assembly</t>
   </si>
   <si>
@@ -249,12 +224,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>V_REG_LD1085D2</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/STMicroelectronics/LD1085D2T-R/?qs=sGAEpiMZZMsGz1a6aV8DcNi9%252bTg6j2AWastsvd5jJkk%3d</t>
-  </si>
-  <si>
     <t>http://www.mouser.com/ProductDetail/Apacer/AP16GMCSH4-B/?qs=sGAEpiMZZMtyMAXUUxCBE4AZ7JbBE3hTRlqQ2Hq7Z8o%3d</t>
   </si>
   <si>
@@ -285,37 +254,43 @@
     <t>BC846-NPN-SOT23-BEC</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/Panasonic/ERJ-2RKF3740X/?qs=sGAEpiMZZMvdGkrng054t8AJgcdMkx7x12YxA1eMwik%3d</t>
-  </si>
-  <si>
-    <t>REORDERS:</t>
-  </si>
-  <si>
-    <t>Shottkey 2A Diode</t>
-  </si>
-  <si>
-    <t>Current protection diode</t>
-  </si>
-  <si>
-    <t>ALTERNATE</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/STMicroelectronics/STPS2150A/?qs=sGAEpiMZZMtQ8nqTKtFS/D9SVzsgHTKGOE6qlz74chY%3d</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/STMicroelectronics/STPS2L60A/?qs=sGAEpiMZZMtQ8nqTKtFS/BdOQ7hRVdjrRRcw/Z2mnfk%3d</t>
-  </si>
-  <si>
     <t>http://www.mouser.com/ProductDetail/Nichicon/UWT1V101MCL1GS/?qs=sGAEpiMZZMtZ1n0r9vR22RxmuzErLMSVBmnA2mTwl6Q%3d</t>
   </si>
   <si>
     <t>http://www.mouser.com/ProductDetail/Panasonic/EEE-FTH101XAP/?qs=sGAEpiMZZMtZ1n0r9vR22faLJZo9l6aZd9hc%252bS3UNLs%3d</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-Semiconductors/MURS360-E3-57T/?qs=sGAEpiMZZMtbRapU8LlZD0HbIjlpuZ44mWs6%252bcqziqw%3d</t>
+  </si>
+  <si>
+    <t>PTC</t>
+  </si>
+  <si>
+    <t>Motor Fuses</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Bourns/MF-SMDF050-2/?qs=sGAEpiMZZMsZt0HrY5I79rMmbkJIXavZ9p5iDdfJTwk%3d</t>
+  </si>
+  <si>
+    <t>V_REG_LD1085</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/STMicroelectronics/LD1085V50/?qs=sGAEpiMZZMsGz1a6aV8DcCRy2MVkeVbmq8UhGP29P1g%3d</t>
+  </si>
+  <si>
+    <t>Molex 2 Wire Jumper assembly</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9918</t>
+  </si>
+  <si>
+    <t>Limit switches @ board and Power/Motor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,7 +347,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -387,6 +362,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -467,6 +443,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -514,7 +493,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -547,9 +526,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -582,6 +578,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -758,24 +771,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="30.265625" style="3" customWidth="1"/>
     <col min="2" max="2" width="30" style="3" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="3"/>
+    <col min="3" max="3" width="32.1328125" style="3"/>
     <col min="4" max="4" width="26" style="3" customWidth="1"/>
-    <col min="5" max="5" width="139.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="123.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="139.265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="123.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,13 +799,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -803,18 +816,21 @@
         <v>6</v>
       </c>
       <c r="D2" s="3">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -823,465 +839,389 @@
         <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="3">
         <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="3">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="3">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="D14" s="3">
+        <v>36</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="3" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="3">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="D15" s="3">
+        <v>36</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="3">
-        <v>12</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="D17" s="3">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="3" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="B18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="3">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="D18" s="3">
+        <v>25</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="B20" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="3">
-        <v>25</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="3">
-        <v>25</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="D20" s="3">
         <v>25</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="3">
+        <v>25</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="3">
+        <v>10</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="D21" s="3">
-        <v>10</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="3">
-        <v>25</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D23" s="3">
         <v>25</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D24" s="3">
         <v>25</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="3">
-        <v>25</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="3">
-        <v>15</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D29" s="3">
         <v>10</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B30" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D30" s="3">
         <v>10</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="3">
-        <v>5</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="3">
+        <v>50</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="3">
+        <v>10</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D34" s="3">
         <v>2</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D35" s="3">
         <v>2</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="3">
-        <v>8</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="3">
-        <v>8</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>97</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2"/>
-    <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E7" r:id="rId4"/>
-    <hyperlink ref="E8" r:id="rId5"/>
-    <hyperlink ref="E9" r:id="rId6"/>
-    <hyperlink ref="E10" r:id="rId7"/>
-    <hyperlink ref="E13" r:id="rId8"/>
-    <hyperlink ref="E14" r:id="rId9"/>
-    <hyperlink ref="E16" r:id="rId10"/>
-    <hyperlink ref="E19" r:id="rId11"/>
-    <hyperlink ref="E20" r:id="rId12"/>
-    <hyperlink ref="E21" r:id="rId13"/>
+    <hyperlink ref="E6" r:id="rId1"/>
+    <hyperlink ref="E7" r:id="rId2"/>
+    <hyperlink ref="E8" r:id="rId3"/>
+    <hyperlink ref="E9" r:id="rId4"/>
+    <hyperlink ref="E10" r:id="rId5"/>
+    <hyperlink ref="E14" r:id="rId6"/>
+    <hyperlink ref="E15" r:id="rId7"/>
+    <hyperlink ref="E17" r:id="rId8"/>
+    <hyperlink ref="E20" r:id="rId9"/>
+    <hyperlink ref="E21" r:id="rId10"/>
+    <hyperlink ref="E22" r:id="rId11"/>
+    <hyperlink ref="E24" r:id="rId12"/>
+    <hyperlink ref="E29" r:id="rId13"/>
     <hyperlink ref="E23" r:id="rId14"/>
-    <hyperlink ref="E25" r:id="rId15"/>
-    <hyperlink ref="E29" r:id="rId16"/>
-    <hyperlink ref="E22" r:id="rId17"/>
-    <hyperlink ref="E28" r:id="rId18"/>
-    <hyperlink ref="E30" r:id="rId19"/>
-    <hyperlink ref="E32" r:id="rId20"/>
-    <hyperlink ref="E34" r:id="rId21"/>
-    <hyperlink ref="E35" r:id="rId22"/>
-    <hyperlink ref="E36" r:id="rId23"/>
-    <hyperlink ref="E17" r:id="rId24"/>
-    <hyperlink ref="E3" r:id="rId25"/>
-    <hyperlink ref="E4" r:id="rId26"/>
+    <hyperlink ref="E30" r:id="rId15"/>
+    <hyperlink ref="E34" r:id="rId16"/>
+    <hyperlink ref="E35" r:id="rId17"/>
+    <hyperlink ref="E36" r:id="rId18"/>
+    <hyperlink ref="E18" r:id="rId19"/>
+    <hyperlink ref="E3" r:id="rId20"/>
+    <hyperlink ref="E4" r:id="rId21"/>
+    <hyperlink ref="E5" r:id="rId22"/>
+    <hyperlink ref="E2" r:id="rId23"/>
+    <hyperlink ref="E33" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -1291,9 +1231,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.59765625"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1307,9 +1247,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125"/>
+    <col min="1" max="1025" width="8.59765625"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>